<commit_message>
added postman api documentation
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log_2023.xlsx
+++ b/DTT-Assessment-Hour-Log_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\bit-academy\Stage\Kwallificerende stage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\bit-academy\Stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FA9CC09-7242-4AC8-9986-F559A59688FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EA6FA65-85CC-436D-8F4A-8696AFBFDFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5856" yWindow="0" windowWidth="17280" windowHeight="12336" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>When creating the factories, it took a long bit before i could seed the data properly inside of the database. I resolved the issue by adjusting my initial sql database setup</t>
+  </si>
+  <si>
+    <t>Createing Search function</t>
+  </si>
+  <si>
+    <t>Added Pagination</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>I used the where clause methods to retrieve the facility information with multiple search queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> created a pagination method to be used for api request</t>
   </si>
 </sst>
 </file>
@@ -841,7 +856,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.53515625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -994,19 +1009,39 @@
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7">
+        <v>45561</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
+      <c r="A11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45561</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -1159,7 +1194,7 @@
       </c>
       <c r="B30" s="14">
         <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>

</xml_diff>